<commit_message>
nmv 15 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.4 Padam Input Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Padam Input Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C205338-1459-4362-94D7-464067F60279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96D442D-2C44-4A11-9B3E-C98D564FBFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS 4.4" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 4.4'!$C$1:$V$1888</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -4502,9 +4494,6 @@
     <t>saha#svataq itiq saha#svate</t>
   </si>
   <si>
-    <t>etyA</t>
-  </si>
-  <si>
     <t>Baqreti# Bara</t>
   </si>
   <si>
@@ -4713,6 +4702,9 @@
   </si>
   <si>
     <t>viSvayuH pAhi??</t>
+  </si>
+  <si>
+    <t>PRE</t>
   </si>
 </sst>
 </file>
@@ -5330,9 +5322,9 @@
   <dimension ref="A1:V1888"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1870" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="S194" sqref="S194"/>
+      <selection pane="bottomLeft" activeCell="N1889" sqref="N1889"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -13210,7 +13202,7 @@
         <v>40</v>
       </c>
       <c r="N184" s="16" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="O184" s="6"/>
       <c r="P184" s="7"/>
@@ -15334,7 +15326,7 @@
         <v>93</v>
       </c>
       <c r="N237" s="20" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="O237" s="7" t="s">
         <v>0</v>
@@ -18632,7 +18624,7 @@
         <v>34</v>
       </c>
       <c r="N318" s="20" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="O318" s="6"/>
       <c r="P318" s="7"/>
@@ -31417,7 +31409,6 @@
       <c r="N627" s="50" t="s">
         <v>513</v>
       </c>
-      <c r="O627" s="6"/>
       <c r="P627" s="7"/>
       <c r="Q627" s="7"/>
       <c r="R627" s="7"/>
@@ -31460,7 +31451,9 @@
       <c r="N628" s="20" t="s">
         <v>518</v>
       </c>
-      <c r="O628" s="6"/>
+      <c r="O628" s="45" t="s">
+        <v>1558</v>
+      </c>
       <c r="P628" s="7" t="s">
         <v>18</v>
       </c>
@@ -31469,9 +31462,7 @@
       <c r="S628" s="7"/>
       <c r="T628" s="7"/>
       <c r="U628" s="7"/>
-      <c r="V628" s="20" t="s">
-        <v>1488</v>
-      </c>
+      <c r="V628" s="20"/>
     </row>
     <row r="629" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A629" s="7"/>
@@ -31851,7 +31842,7 @@
       <c r="T637" s="7"/>
       <c r="U637" s="7"/>
       <c r="V637" s="20" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="638" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -32187,7 +32178,7 @@
       <c r="T645" s="7"/>
       <c r="U645" s="7"/>
       <c r="V645" s="20" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="646" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -32482,7 +32473,7 @@
       <c r="T652" s="7"/>
       <c r="U652" s="7"/>
       <c r="V652" s="20" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="653" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -32781,7 +32772,7 @@
       <c r="T659" s="7"/>
       <c r="U659" s="7"/>
       <c r="V659" s="20" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="660" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -33079,7 +33070,7 @@
       <c r="T666" s="7"/>
       <c r="U666" s="7"/>
       <c r="V666" s="20" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="667" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -33345,7 +33336,7 @@
       <c r="T672" s="7"/>
       <c r="U672" s="7"/>
       <c r="V672" s="20" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="673" spans="1:22" x14ac:dyDescent="0.25">
@@ -33689,7 +33680,7 @@
       <c r="T680" s="7"/>
       <c r="U680" s="7"/>
       <c r="V680" s="20" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="681" spans="1:22" x14ac:dyDescent="0.25">
@@ -33945,7 +33936,7 @@
       <c r="T686" s="7"/>
       <c r="U686" s="7"/>
       <c r="V686" s="20" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="687" spans="1:22" x14ac:dyDescent="0.25">
@@ -34162,7 +34153,7 @@
       <c r="T691" s="7"/>
       <c r="U691" s="7"/>
       <c r="V691" s="20" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="692" spans="1:22" x14ac:dyDescent="0.25">
@@ -34465,7 +34456,7 @@
       <c r="T698" s="7"/>
       <c r="U698" s="7"/>
       <c r="V698" s="20" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="699" spans="1:22" x14ac:dyDescent="0.25">
@@ -34641,7 +34632,7 @@
       <c r="T702" s="7"/>
       <c r="U702" s="7"/>
       <c r="V702" s="20" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="703" spans="1:22" x14ac:dyDescent="0.25">
@@ -34973,7 +34964,7 @@
       <c r="T710" s="7"/>
       <c r="U710" s="7"/>
       <c r="V710" s="20" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="711" spans="1:22" x14ac:dyDescent="0.25">
@@ -35187,7 +35178,7 @@
       <c r="T715" s="7"/>
       <c r="U715" s="7"/>
       <c r="V715" s="20" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="716" spans="1:22" x14ac:dyDescent="0.25">
@@ -35486,7 +35477,7 @@
       <c r="T722" s="7"/>
       <c r="U722" s="7"/>
       <c r="V722" s="20" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="723" spans="1:22" x14ac:dyDescent="0.25">
@@ -36004,7 +35995,7 @@
       <c r="T734" s="7"/>
       <c r="U734" s="7"/>
       <c r="V734" s="20" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="735" spans="1:22" x14ac:dyDescent="0.25">
@@ -36358,7 +36349,7 @@
       <c r="T742" s="7"/>
       <c r="U742" s="7"/>
       <c r="V742" s="20" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="743" spans="1:22" x14ac:dyDescent="0.25">
@@ -36786,7 +36777,7 @@
       <c r="T752" s="7"/>
       <c r="U752" s="7"/>
       <c r="V752" s="20" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="753" spans="1:22" x14ac:dyDescent="0.25">
@@ -37048,7 +37039,7 @@
       <c r="T758" s="7"/>
       <c r="U758" s="7"/>
       <c r="V758" s="20" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="759" spans="1:22" x14ac:dyDescent="0.25">
@@ -37530,7 +37521,7 @@
       <c r="T769" s="7"/>
       <c r="U769" s="7"/>
       <c r="V769" s="20" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="770" spans="1:22" x14ac:dyDescent="0.25">
@@ -37962,7 +37953,7 @@
       <c r="T779" s="7"/>
       <c r="U779" s="7"/>
       <c r="V779" s="20" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="780" spans="1:22" x14ac:dyDescent="0.25">
@@ -38091,7 +38082,7 @@
       <c r="T782" s="7"/>
       <c r="U782" s="7"/>
       <c r="V782" s="20" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="783" spans="1:22" x14ac:dyDescent="0.25">
@@ -38398,7 +38389,7 @@
       <c r="T789" s="7"/>
       <c r="U789" s="7"/>
       <c r="V789" s="20" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="790" spans="1:22" x14ac:dyDescent="0.25">
@@ -38566,7 +38557,7 @@
       <c r="T793" s="7"/>
       <c r="U793" s="7"/>
       <c r="V793" s="20" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="794" spans="1:22" x14ac:dyDescent="0.25">
@@ -38871,7 +38862,7 @@
       <c r="T800" s="7"/>
       <c r="U800" s="7"/>
       <c r="V800" s="20" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="801" spans="1:22" x14ac:dyDescent="0.25">
@@ -39123,7 +39114,7 @@
       <c r="T806" s="7"/>
       <c r="U806" s="7"/>
       <c r="V806" s="20" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="807" spans="1:22" x14ac:dyDescent="0.25">
@@ -39505,7 +39496,7 @@
       <c r="T815" s="7"/>
       <c r="U815" s="7"/>
       <c r="V815" s="20" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="816" spans="1:22" x14ac:dyDescent="0.25">
@@ -39677,7 +39668,7 @@
       <c r="T819" s="7"/>
       <c r="U819" s="7"/>
       <c r="V819" s="20" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="820" spans="1:22" x14ac:dyDescent="0.25">
@@ -40011,7 +40002,7 @@
       <c r="T827" s="7"/>
       <c r="U827" s="7"/>
       <c r="V827" s="20" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="828" spans="1:22" x14ac:dyDescent="0.25">
@@ -40140,7 +40131,7 @@
       <c r="T830" s="7"/>
       <c r="U830" s="7"/>
       <c r="V830" s="20" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="831" spans="1:22" x14ac:dyDescent="0.25">
@@ -40394,7 +40385,7 @@
       <c r="T836" s="7"/>
       <c r="U836" s="7"/>
       <c r="V836" s="20" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="837" spans="1:22" x14ac:dyDescent="0.25">
@@ -40487,7 +40478,7 @@
     </row>
     <row r="839" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A839" s="16" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="B839" s="28"/>
       <c r="C839" s="38" t="s">
@@ -40668,7 +40659,7 @@
       <c r="T842" s="7"/>
       <c r="U842" s="7"/>
       <c r="V842" s="20" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="843" spans="1:22" x14ac:dyDescent="0.25">
@@ -40854,7 +40845,7 @@
         <v>119</v>
       </c>
       <c r="V846" s="20" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="847" spans="1:22" x14ac:dyDescent="0.25">
@@ -41063,7 +41054,7 @@
       <c r="T851" s="7"/>
       <c r="U851" s="7"/>
       <c r="V851" s="20" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="852" spans="1:22" x14ac:dyDescent="0.25">
@@ -41231,7 +41222,7 @@
       <c r="T855" s="7"/>
       <c r="U855" s="7"/>
       <c r="V855" s="20" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="856" spans="1:22" x14ac:dyDescent="0.25">
@@ -41401,7 +41392,7 @@
       <c r="T859" s="7"/>
       <c r="U859" s="7"/>
       <c r="V859" s="20" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="860" spans="1:22" x14ac:dyDescent="0.25">
@@ -41530,7 +41521,7 @@
       <c r="T862" s="7"/>
       <c r="U862" s="7"/>
       <c r="V862" s="20" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="863" spans="1:22" x14ac:dyDescent="0.25">
@@ -41747,7 +41738,7 @@
       <c r="T867" s="7"/>
       <c r="U867" s="7"/>
       <c r="V867" s="20" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="868" spans="1:22" x14ac:dyDescent="0.25">
@@ -45640,7 +45631,7 @@
       <c r="T965" s="7"/>
       <c r="U965" s="7"/>
       <c r="V965" s="20" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="966" spans="1:22" x14ac:dyDescent="0.25">
@@ -52951,7 +52942,7 @@
     </row>
     <row r="1148" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1148" s="7" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="B1148" s="28"/>
       <c r="C1148" s="28"/>
@@ -54127,7 +54118,7 @@
       <c r="T1176" s="7"/>
       <c r="U1176" s="7"/>
       <c r="V1176" s="20" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="1177" spans="1:22" x14ac:dyDescent="0.25">
@@ -56106,7 +56097,7 @@
       <c r="T1225" s="7"/>
       <c r="U1225" s="7"/>
       <c r="V1225" s="20" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="1226" spans="1:22" x14ac:dyDescent="0.25">
@@ -59065,7 +59056,7 @@
       <c r="T1296" s="7"/>
       <c r="U1296" s="7"/>
       <c r="V1296" s="20" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="1297" spans="1:22" x14ac:dyDescent="0.25">
@@ -64322,7 +64313,7 @@
       <c r="T1429" s="7"/>
       <c r="U1429" s="7"/>
       <c r="V1429" s="20" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="1430" spans="1:22" x14ac:dyDescent="0.25">
@@ -66255,7 +66246,7 @@
         <v>49</v>
       </c>
       <c r="N1478" s="20" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="O1478" s="6"/>
       <c r="P1478" s="7"/>
@@ -71127,7 +71118,7 @@
         <v>18</v>
       </c>
       <c r="V1624" s="20" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="1625" spans="1:22" x14ac:dyDescent="0.25">
@@ -71422,7 +71413,7 @@
         <v>18</v>
       </c>
       <c r="V1634" s="20" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="1635" spans="3:22" x14ac:dyDescent="0.25">
@@ -71676,7 +71667,7 @@
         <v>18</v>
       </c>
       <c r="V1643" s="20" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="1644" spans="3:22" x14ac:dyDescent="0.25">
@@ -71883,7 +71874,7 @@
         <v>18</v>
       </c>
       <c r="V1650" s="20" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="1651" spans="3:22" x14ac:dyDescent="0.25">
@@ -72171,7 +72162,7 @@
         <v>18</v>
       </c>
       <c r="V1660" s="20" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="1661" spans="3:22" x14ac:dyDescent="0.25">
@@ -72405,7 +72396,7 @@
         <v>18</v>
       </c>
       <c r="V1668" s="20" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="1669" spans="3:22" x14ac:dyDescent="0.25">
@@ -72693,7 +72684,7 @@
         <v>18</v>
       </c>
       <c r="V1678" s="20" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="1679" spans="3:22" x14ac:dyDescent="0.25">
@@ -72927,7 +72918,7 @@
         <v>18</v>
       </c>
       <c r="V1686" s="20" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="1687" spans="3:22" x14ac:dyDescent="0.25">
@@ -73153,7 +73144,7 @@
         <v>18</v>
       </c>
       <c r="V1694" s="20" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="1695" spans="3:22" x14ac:dyDescent="0.25">
@@ -73638,7 +73629,7 @@
         <v>18</v>
       </c>
       <c r="V1711" s="20" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="1712" spans="3:22" x14ac:dyDescent="0.25">
@@ -73916,7 +73907,7 @@
         <v>18</v>
       </c>
       <c r="V1721" s="20" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="1722" spans="3:22" x14ac:dyDescent="0.25">
@@ -74146,7 +74137,7 @@
         <v>18</v>
       </c>
       <c r="V1729" s="20" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="1730" spans="3:22" x14ac:dyDescent="0.25">
@@ -74434,7 +74425,7 @@
         <v>18</v>
       </c>
       <c r="V1739" s="20" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="1740" spans="3:22" x14ac:dyDescent="0.25">
@@ -74692,7 +74683,7 @@
         <v>18</v>
       </c>
       <c r="V1748" s="20" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="1749" spans="3:22" x14ac:dyDescent="0.25">
@@ -74968,7 +74959,7 @@
         <v>18</v>
       </c>
       <c r="V1757" s="20" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="1758" spans="3:22" x14ac:dyDescent="0.25">
@@ -75443,7 +75434,7 @@
         <v>18</v>
       </c>
       <c r="V1773" s="20" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="1774" spans="3:22" x14ac:dyDescent="0.25">
@@ -75707,7 +75698,7 @@
         <v>18</v>
       </c>
       <c r="V1782" s="20" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="1783" spans="3:22" x14ac:dyDescent="0.25">
@@ -75980,7 +75971,7 @@
         <v>18</v>
       </c>
       <c r="V1791" s="20" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="1792" spans="3:22" x14ac:dyDescent="0.25">
@@ -76253,7 +76244,7 @@
         <v>18</v>
       </c>
       <c r="V1800" s="20" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="1801" spans="3:22" x14ac:dyDescent="0.25">
@@ -76509,7 +76500,7 @@
         <v>119</v>
       </c>
       <c r="V1809" s="20" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="1810" spans="3:22" x14ac:dyDescent="0.25">
@@ -76788,7 +76779,7 @@
         <v>119</v>
       </c>
       <c r="V1818" s="20" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="1819" spans="3:22" x14ac:dyDescent="0.25">
@@ -76997,7 +76988,7 @@
         <v>18</v>
       </c>
       <c r="V1825" s="20" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="1826" spans="3:22" x14ac:dyDescent="0.25">
@@ -77252,7 +77243,7 @@
         <v>119</v>
       </c>
       <c r="V1833" s="20" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="1834" spans="3:22" x14ac:dyDescent="0.25">
@@ -77520,7 +77511,7 @@
         <v>18</v>
       </c>
       <c r="V1842" s="20" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="1843" spans="3:22" x14ac:dyDescent="0.25">
@@ -77654,13 +77645,13 @@
         <v>223</v>
       </c>
       <c r="N1847" s="20" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="O1847" s="7" t="s">
         <v>0</v>
       </c>
       <c r="V1847" s="20" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="1848" spans="3:22" x14ac:dyDescent="0.25">
@@ -77779,7 +77770,7 @@
         <v>18</v>
       </c>
       <c r="V1851" s="20" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="1852" spans="3:22" x14ac:dyDescent="0.25">
@@ -78248,7 +78239,7 @@
         <v>18</v>
       </c>
       <c r="V1867" s="20" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="1868" spans="3:22" x14ac:dyDescent="0.25">
@@ -78887,7 +78878,7 @@
         <v>18</v>
       </c>
       <c r="V1888" s="20" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nmv 19 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC8E1B2-4228-48EB-9774-9713B5A288F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF5F359-E5D8-42EC-8CAA-7028FD9BFAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5789" uniqueCount="1557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5794" uniqueCount="1556">
   <si>
     <t>PS</t>
   </si>
@@ -4522,9 +4522,6 @@
   </si>
   <si>
     <t>aqjaraqmityaqjara$m</t>
-  </si>
-  <si>
-    <t>Baqreqti# Bara</t>
   </si>
   <si>
     <t>paqtaq iti# pate</t>
@@ -5318,10 +5315,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1888"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A477" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A777" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="S491" sqref="S491"/>
+      <selection pane="bottomLeft" activeCell="N794" sqref="N794"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -13199,7 +13196,7 @@
         <v>40</v>
       </c>
       <c r="N184" s="16" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="O184" s="6"/>
       <c r="P184" s="7"/>
@@ -15323,7 +15320,7 @@
         <v>93</v>
       </c>
       <c r="N237" s="20" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="O237" s="7" t="s">
         <v>0</v>
@@ -15974,7 +15971,7 @@
       <c r="T253" s="7"/>
       <c r="U253" s="7"/>
       <c r="V253" s="16" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="254" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -16060,7 +16057,7 @@
       <c r="T255" s="7"/>
       <c r="U255" s="7"/>
       <c r="V255" s="16" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="256" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -18621,7 +18618,7 @@
         <v>34</v>
       </c>
       <c r="N318" s="20" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="O318" s="6"/>
       <c r="P318" s="7"/>
@@ -29247,8 +29244,12 @@
       <c r="P576" s="7"/>
       <c r="Q576" s="7"/>
       <c r="R576" s="7"/>
-      <c r="S576" s="7"/>
-      <c r="T576" s="7"/>
+      <c r="S576" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T576" s="54" t="s">
+        <v>124</v>
+      </c>
       <c r="U576" s="7"/>
       <c r="V576" s="20"/>
     </row>
@@ -31453,7 +31454,7 @@
         <v>516</v>
       </c>
       <c r="O628" s="45" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="P628" s="7" t="s">
         <v>18</v>
@@ -34369,7 +34370,9 @@
       <c r="R696" s="7"/>
       <c r="S696" s="7"/>
       <c r="T696" s="7"/>
-      <c r="U696" s="7"/>
+      <c r="U696" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="V696" s="20"/>
     </row>
     <row r="697" spans="1:22" x14ac:dyDescent="0.25">
@@ -35995,8 +35998,8 @@
       <c r="S734" s="7"/>
       <c r="T734" s="7"/>
       <c r="U734" s="7"/>
-      <c r="V734" s="20" t="s">
-        <v>1498</v>
+      <c r="V734" s="16" t="s">
+        <v>1484</v>
       </c>
     </row>
     <row r="735" spans="1:22" x14ac:dyDescent="0.25">
@@ -36350,7 +36353,7 @@
       <c r="T742" s="7"/>
       <c r="U742" s="7"/>
       <c r="V742" s="20" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="743" spans="1:22" x14ac:dyDescent="0.25">
@@ -37040,7 +37043,7 @@
       <c r="T758" s="7"/>
       <c r="U758" s="7"/>
       <c r="V758" s="20" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="759" spans="1:22" x14ac:dyDescent="0.25">
@@ -37521,8 +37524,8 @@
       <c r="S769" s="7"/>
       <c r="T769" s="7"/>
       <c r="U769" s="7"/>
-      <c r="V769" s="20" t="s">
-        <v>1498</v>
+      <c r="V769" s="16" t="s">
+        <v>1484</v>
       </c>
     </row>
     <row r="770" spans="1:22" x14ac:dyDescent="0.25">
@@ -37954,7 +37957,7 @@
       <c r="T779" s="7"/>
       <c r="U779" s="7"/>
       <c r="V779" s="20" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="780" spans="1:22" x14ac:dyDescent="0.25">
@@ -38083,7 +38086,7 @@
       <c r="T782" s="7"/>
       <c r="U782" s="7"/>
       <c r="V782" s="20" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="783" spans="1:22" x14ac:dyDescent="0.25">
@@ -38390,7 +38393,7 @@
       <c r="T789" s="7"/>
       <c r="U789" s="7"/>
       <c r="V789" s="20" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="790" spans="1:22" x14ac:dyDescent="0.25">
@@ -38554,11 +38557,9 @@
       </c>
       <c r="Q793" s="7"/>
       <c r="R793" s="7"/>
-      <c r="S793" s="7"/>
-      <c r="T793" s="7"/>
       <c r="U793" s="7"/>
       <c r="V793" s="20" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="794" spans="1:22" x14ac:dyDescent="0.25">
@@ -38599,8 +38600,12 @@
       <c r="P794" s="7"/>
       <c r="Q794" s="7"/>
       <c r="R794" s="7"/>
-      <c r="S794" s="7"/>
-      <c r="T794" s="7"/>
+      <c r="S794" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T794" s="7" t="s">
+        <v>114</v>
+      </c>
       <c r="U794" s="7"/>
       <c r="V794" s="20"/>
     </row>
@@ -38863,7 +38868,7 @@
       <c r="T800" s="7"/>
       <c r="U800" s="7"/>
       <c r="V800" s="20" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="801" spans="1:22" x14ac:dyDescent="0.25">
@@ -39115,7 +39120,7 @@
       <c r="T806" s="7"/>
       <c r="U806" s="7"/>
       <c r="V806" s="20" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="807" spans="1:22" x14ac:dyDescent="0.25">
@@ -39497,7 +39502,7 @@
       <c r="T815" s="7"/>
       <c r="U815" s="7"/>
       <c r="V815" s="20" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="816" spans="1:22" x14ac:dyDescent="0.25">
@@ -39669,7 +39674,7 @@
       <c r="T819" s="7"/>
       <c r="U819" s="7"/>
       <c r="V819" s="20" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="820" spans="1:22" x14ac:dyDescent="0.25">
@@ -40003,7 +40008,7 @@
       <c r="T827" s="7"/>
       <c r="U827" s="7"/>
       <c r="V827" s="20" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="828" spans="1:22" x14ac:dyDescent="0.25">
@@ -40132,7 +40137,7 @@
       <c r="T830" s="7"/>
       <c r="U830" s="7"/>
       <c r="V830" s="20" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="831" spans="1:22" x14ac:dyDescent="0.25">
@@ -40386,7 +40391,7 @@
       <c r="T836" s="7"/>
       <c r="U836" s="7"/>
       <c r="V836" s="20" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="837" spans="1:22" x14ac:dyDescent="0.25">
@@ -40479,7 +40484,7 @@
     </row>
     <row r="839" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A839" s="16" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="B839" s="28"/>
       <c r="C839" s="38" t="s">
@@ -40660,7 +40665,7 @@
       <c r="T842" s="7"/>
       <c r="U842" s="7"/>
       <c r="V842" s="20" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="843" spans="1:22" x14ac:dyDescent="0.25">
@@ -40846,7 +40851,7 @@
         <v>119</v>
       </c>
       <c r="V846" s="20" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="847" spans="1:22" x14ac:dyDescent="0.25">
@@ -41055,7 +41060,7 @@
       <c r="T851" s="7"/>
       <c r="U851" s="7"/>
       <c r="V851" s="20" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="852" spans="1:22" x14ac:dyDescent="0.25">
@@ -41223,7 +41228,7 @@
       <c r="T855" s="7"/>
       <c r="U855" s="7"/>
       <c r="V855" s="20" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="856" spans="1:22" x14ac:dyDescent="0.25">
@@ -41393,7 +41398,7 @@
       <c r="T859" s="7"/>
       <c r="U859" s="7"/>
       <c r="V859" s="20" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="860" spans="1:22" x14ac:dyDescent="0.25">
@@ -41522,7 +41527,7 @@
       <c r="T862" s="7"/>
       <c r="U862" s="7"/>
       <c r="V862" s="20" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="863" spans="1:22" x14ac:dyDescent="0.25">
@@ -41739,7 +41744,7 @@
       <c r="T867" s="7"/>
       <c r="U867" s="7"/>
       <c r="V867" s="20" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="868" spans="1:22" x14ac:dyDescent="0.25">
@@ -45632,7 +45637,7 @@
       <c r="T965" s="7"/>
       <c r="U965" s="7"/>
       <c r="V965" s="20" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="966" spans="1:22" x14ac:dyDescent="0.25">
@@ -52943,7 +52948,7 @@
     </row>
     <row r="1148" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1148" s="7" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="B1148" s="28"/>
       <c r="C1148" s="28"/>
@@ -54119,7 +54124,7 @@
       <c r="T1176" s="7"/>
       <c r="U1176" s="7"/>
       <c r="V1176" s="20" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="1177" spans="1:22" x14ac:dyDescent="0.25">
@@ -56098,7 +56103,7 @@
       <c r="T1225" s="7"/>
       <c r="U1225" s="7"/>
       <c r="V1225" s="20" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="1226" spans="1:22" x14ac:dyDescent="0.25">
@@ -59057,7 +59062,7 @@
       <c r="T1296" s="7"/>
       <c r="U1296" s="7"/>
       <c r="V1296" s="20" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="1297" spans="1:22" x14ac:dyDescent="0.25">
@@ -64314,7 +64319,7 @@
       <c r="T1429" s="7"/>
       <c r="U1429" s="7"/>
       <c r="V1429" s="20" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="1430" spans="1:22" x14ac:dyDescent="0.25">
@@ -66247,7 +66252,7 @@
         <v>49</v>
       </c>
       <c r="N1478" s="20" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="O1478" s="6"/>
       <c r="P1478" s="7"/>
@@ -71119,7 +71124,7 @@
         <v>18</v>
       </c>
       <c r="V1624" s="20" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="1625" spans="1:22" x14ac:dyDescent="0.25">
@@ -71414,7 +71419,7 @@
         <v>18</v>
       </c>
       <c r="V1634" s="20" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="1635" spans="3:22" x14ac:dyDescent="0.25">
@@ -71668,7 +71673,7 @@
         <v>18</v>
       </c>
       <c r="V1643" s="20" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="1644" spans="3:22" x14ac:dyDescent="0.25">
@@ -71875,7 +71880,7 @@
         <v>18</v>
       </c>
       <c r="V1650" s="20" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="1651" spans="3:22" x14ac:dyDescent="0.25">
@@ -72163,7 +72168,7 @@
         <v>18</v>
       </c>
       <c r="V1660" s="20" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="1661" spans="3:22" x14ac:dyDescent="0.25">
@@ -72397,7 +72402,7 @@
         <v>18</v>
       </c>
       <c r="V1668" s="20" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="1669" spans="3:22" x14ac:dyDescent="0.25">
@@ -72685,7 +72690,7 @@
         <v>18</v>
       </c>
       <c r="V1678" s="20" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="1679" spans="3:22" x14ac:dyDescent="0.25">
@@ -72919,7 +72924,7 @@
         <v>18</v>
       </c>
       <c r="V1686" s="20" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="1687" spans="3:22" x14ac:dyDescent="0.25">
@@ -73145,7 +73150,7 @@
         <v>18</v>
       </c>
       <c r="V1694" s="20" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="1695" spans="3:22" x14ac:dyDescent="0.25">
@@ -73630,7 +73635,7 @@
         <v>18</v>
       </c>
       <c r="V1711" s="20" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="1712" spans="3:22" x14ac:dyDescent="0.25">
@@ -73908,7 +73913,7 @@
         <v>18</v>
       </c>
       <c r="V1721" s="20" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="1722" spans="3:22" x14ac:dyDescent="0.25">
@@ -74138,7 +74143,7 @@
         <v>18</v>
       </c>
       <c r="V1729" s="20" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="1730" spans="3:22" x14ac:dyDescent="0.25">
@@ -74426,7 +74431,7 @@
         <v>18</v>
       </c>
       <c r="V1739" s="20" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="1740" spans="3:22" x14ac:dyDescent="0.25">
@@ -74684,7 +74689,7 @@
         <v>18</v>
       </c>
       <c r="V1748" s="20" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="1749" spans="3:22" x14ac:dyDescent="0.25">
@@ -74960,7 +74965,7 @@
         <v>18</v>
       </c>
       <c r="V1757" s="20" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="1758" spans="3:22" x14ac:dyDescent="0.25">
@@ -75435,7 +75440,7 @@
         <v>18</v>
       </c>
       <c r="V1773" s="20" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="1774" spans="3:22" x14ac:dyDescent="0.25">
@@ -75699,7 +75704,7 @@
         <v>18</v>
       </c>
       <c r="V1782" s="20" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="1783" spans="3:22" x14ac:dyDescent="0.25">
@@ -75972,7 +75977,7 @@
         <v>18</v>
       </c>
       <c r="V1791" s="20" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="1792" spans="3:22" x14ac:dyDescent="0.25">
@@ -76245,7 +76250,7 @@
         <v>18</v>
       </c>
       <c r="V1800" s="20" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="1801" spans="3:22" x14ac:dyDescent="0.25">
@@ -76501,7 +76506,7 @@
         <v>119</v>
       </c>
       <c r="V1809" s="20" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="1810" spans="3:22" x14ac:dyDescent="0.25">
@@ -76780,7 +76785,7 @@
         <v>119</v>
       </c>
       <c r="V1818" s="20" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="1819" spans="3:22" x14ac:dyDescent="0.25">
@@ -76989,7 +76994,7 @@
         <v>18</v>
       </c>
       <c r="V1825" s="20" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="1826" spans="3:22" x14ac:dyDescent="0.25">
@@ -77244,7 +77249,7 @@
         <v>119</v>
       </c>
       <c r="V1833" s="20" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="1834" spans="3:22" x14ac:dyDescent="0.25">
@@ -77512,7 +77517,7 @@
         <v>18</v>
       </c>
       <c r="V1842" s="20" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="1843" spans="3:22" x14ac:dyDescent="0.25">
@@ -77646,13 +77651,13 @@
         <v>223</v>
       </c>
       <c r="N1847" s="20" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="O1847" s="7" t="s">
         <v>0</v>
       </c>
       <c r="V1847" s="20" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="1848" spans="3:22" x14ac:dyDescent="0.25">
@@ -77771,7 +77776,7 @@
         <v>18</v>
       </c>
       <c r="V1851" s="20" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="1852" spans="3:22" x14ac:dyDescent="0.25">
@@ -78240,7 +78245,7 @@
         <v>18</v>
       </c>
       <c r="V1867" s="20" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="1868" spans="3:22" x14ac:dyDescent="0.25">
@@ -78879,7 +78884,7 @@
         <v>18</v>
       </c>
       <c r="V1888" s="20" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nmv 20 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF5F359-E5D8-42EC-8CAA-7028FD9BFAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C912A0-6A23-4BB7-9D90-C5F262431062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5316,9 +5316,9 @@
   <dimension ref="A1:V1888"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A777" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A993" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N794" sqref="N794"/>
+      <selection pane="bottomLeft" activeCell="N1012" sqref="N1012"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -47517,8 +47517,8 @@
         <f t="shared" si="83"/>
         <v>47</v>
       </c>
-      <c r="N1012" s="20" t="s">
-        <v>385</v>
+      <c r="N1012" s="16" t="s">
+        <v>141</v>
       </c>
       <c r="O1012" s="7"/>
       <c r="P1012" s="7"/>

</xml_diff>

<commit_message>
nmv 22 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.4 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C912A0-6A23-4BB7-9D90-C5F262431062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9E025F-5757-4DEC-895E-35077A099677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3999,9 +3999,6 @@
     <t>viSA#Keq itiq vi - SAqKeq</t>
   </si>
   <si>
-    <t>i#006C;qdrAqgnI itI$ndra - aqgnI</t>
-  </si>
-  <si>
     <t>aqnUqrAqdhA itya#nu - rAqdhAH</t>
   </si>
   <si>
@@ -4023,9 +4020,6 @@
     <t>aqpaqBara#NIqritya#pa - Bara#NIH</t>
   </si>
   <si>
-    <t>RuqtU iti# RuqtU</t>
-  </si>
-  <si>
     <t>aqntaqHSleqSha itya#ntaH - SleqShaH</t>
   </si>
   <si>
@@ -4696,6 +4690,12 @@
   </si>
   <si>
     <t>avya#thayantIq ityavya#thayantI</t>
+  </si>
+  <si>
+    <t>RuqtU ityRuqtU</t>
+  </si>
+  <si>
+    <t>iqndrAqgnI itI$ndra - aqgnI</t>
   </si>
 </sst>
 </file>
@@ -5316,9 +5316,9 @@
   <dimension ref="A1:V1888"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A993" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N1012" sqref="N1012"/>
+      <selection pane="bottomLeft" activeCell="V1484" sqref="V1484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5955,7 +5955,7 @@
         <v>3</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="O4" s="7"/>
       <c r="P4" s="15"/>
@@ -11610,7 +11610,7 @@
       <c r="T144" s="7"/>
       <c r="U144" s="7"/>
       <c r="V144" s="20" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="145" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -13196,7 +13196,7 @@
         <v>40</v>
       </c>
       <c r="N184" s="16" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
       <c r="O184" s="6"/>
       <c r="P184" s="7"/>
@@ -15320,7 +15320,7 @@
         <v>93</v>
       </c>
       <c r="N237" s="20" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
       <c r="O237" s="7" t="s">
         <v>0</v>
@@ -15971,7 +15971,7 @@
       <c r="T253" s="7"/>
       <c r="U253" s="7"/>
       <c r="V253" s="16" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="254" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -16057,7 +16057,7 @@
       <c r="T255" s="7"/>
       <c r="U255" s="7"/>
       <c r="V255" s="16" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="256" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -17222,7 +17222,7 @@
         <v>140</v>
       </c>
       <c r="N284" s="20" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="O284" s="6"/>
       <c r="P284" s="7" t="s">
@@ -17234,7 +17234,7 @@
       <c r="T284" s="7"/>
       <c r="U284" s="7"/>
       <c r="V284" s="20" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="285" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -18618,7 +18618,7 @@
         <v>34</v>
       </c>
       <c r="N318" s="20" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="O318" s="6"/>
       <c r="P318" s="7"/>
@@ -23547,7 +23547,7 @@
       <c r="T441" s="7"/>
       <c r="U441" s="7"/>
       <c r="V441" s="20" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="442" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -23896,7 +23896,7 @@
         <v>166</v>
       </c>
       <c r="N450" s="20" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="O450" s="7" t="s">
         <v>0</v>
@@ -23910,7 +23910,7 @@
       <c r="T450" s="7"/>
       <c r="U450" s="7"/>
       <c r="V450" s="20" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="451" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -24392,7 +24392,7 @@
         <v>178</v>
       </c>
       <c r="N462" s="20" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="O462" s="6"/>
       <c r="P462" s="7" t="s">
@@ -24404,7 +24404,7 @@
       <c r="T462" s="7"/>
       <c r="U462" s="7"/>
       <c r="V462" s="20" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="463" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -24715,7 +24715,7 @@
       <c r="T469" s="7"/>
       <c r="U469" s="7"/>
       <c r="V469" s="20" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="470" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -24830,7 +24830,7 @@
         <v>10</v>
       </c>
       <c r="N472" s="20" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="O472" s="6"/>
       <c r="P472" s="7" t="s">
@@ -24842,7 +24842,7 @@
       <c r="T472" s="7"/>
       <c r="U472" s="7"/>
       <c r="V472" s="20" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="473" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -25131,7 +25131,7 @@
         <v>17</v>
       </c>
       <c r="N479" s="20" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="O479" s="6"/>
       <c r="P479" s="7" t="s">
@@ -25143,7 +25143,7 @@
       <c r="T479" s="7"/>
       <c r="U479" s="7"/>
       <c r="V479" s="20" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="480" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -25258,7 +25258,7 @@
         <v>20</v>
       </c>
       <c r="N482" s="20" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="O482" s="6"/>
       <c r="P482" s="7" t="s">
@@ -25270,7 +25270,7 @@
       <c r="T482" s="7"/>
       <c r="U482" s="7"/>
       <c r="V482" s="20" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="483" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -25530,7 +25530,7 @@
       </c>
       <c r="U488" s="7"/>
       <c r="V488" s="20" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="489" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -25645,7 +25645,7 @@
         <v>29</v>
       </c>
       <c r="N491" s="20" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="O491" s="6"/>
       <c r="P491" s="7" t="s">
@@ -25657,7 +25657,7 @@
       <c r="T491" s="7"/>
       <c r="U491" s="7"/>
       <c r="V491" s="20" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="492" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -26024,7 +26024,7 @@
         <v>38</v>
       </c>
       <c r="N500" s="20" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="O500" s="6"/>
       <c r="P500" s="7" t="s">
@@ -26036,7 +26036,7 @@
       <c r="T500" s="7"/>
       <c r="U500" s="7"/>
       <c r="V500" s="20" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="501" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -26362,7 +26362,7 @@
         <v>46</v>
       </c>
       <c r="N508" s="20" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="O508" s="7" t="s">
         <v>0</v>
@@ -26376,7 +26376,7 @@
       <c r="T508" s="7"/>
       <c r="U508" s="7"/>
       <c r="V508" s="20" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="509" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -26746,7 +26746,7 @@
         <v>55</v>
       </c>
       <c r="N517" s="20" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="O517" s="6"/>
       <c r="P517" s="7" t="s">
@@ -26758,7 +26758,7 @@
       <c r="T517" s="7"/>
       <c r="U517" s="7"/>
       <c r="V517" s="20" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="518" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -27180,7 +27180,7 @@
       <c r="T527" s="7"/>
       <c r="U527" s="7"/>
       <c r="V527" s="20" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="528" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -27465,7 +27465,7 @@
         <v>72</v>
       </c>
       <c r="N534" s="20" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="O534" s="6"/>
       <c r="P534" s="7" t="s">
@@ -27477,7 +27477,7 @@
       <c r="T534" s="7"/>
       <c r="U534" s="7"/>
       <c r="V534" s="20" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="535" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -27838,7 +27838,7 @@
         <v>81</v>
       </c>
       <c r="N543" s="20" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="O543" s="6"/>
       <c r="P543" s="7" t="s">
@@ -27850,7 +27850,7 @@
       <c r="T543" s="7"/>
       <c r="U543" s="7"/>
       <c r="V543" s="20" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="544" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -28180,7 +28180,7 @@
         <v>89</v>
       </c>
       <c r="N551" s="20" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="O551" s="6"/>
       <c r="P551" s="7" t="s">
@@ -28192,7 +28192,7 @@
       <c r="T551" s="7"/>
       <c r="U551" s="7"/>
       <c r="V551" s="20" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="552" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -28538,7 +28538,7 @@
       <c r="T559" s="7"/>
       <c r="U559" s="7"/>
       <c r="V559" s="20" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="560" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -28904,7 +28904,7 @@
         <v>106</v>
       </c>
       <c r="N568" s="20" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="O568" s="7" t="s">
         <v>0</v>
@@ -28918,7 +28918,7 @@
       <c r="T568" s="7"/>
       <c r="U568" s="7"/>
       <c r="V568" s="20" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="569" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -29324,7 +29324,7 @@
         <v>116</v>
       </c>
       <c r="N578" s="50" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="O578" s="7"/>
       <c r="P578" s="7" t="s">
@@ -29338,7 +29338,7 @@
         <v>120</v>
       </c>
       <c r="V578" s="20" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="579" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -29723,7 +29723,7 @@
       <c r="T587" s="7"/>
       <c r="U587" s="7"/>
       <c r="V587" s="20" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="588" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -30139,7 +30139,7 @@
         <v>135</v>
       </c>
       <c r="N597" s="20" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="O597" s="7" t="s">
         <v>0</v>
@@ -30153,7 +30153,7 @@
       <c r="T597" s="7"/>
       <c r="U597" s="7"/>
       <c r="V597" s="20" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="598" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -30354,7 +30354,7 @@
         <v>140</v>
       </c>
       <c r="N602" s="20" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="O602" s="6"/>
       <c r="P602" s="7" t="s">
@@ -30366,7 +30366,7 @@
       <c r="T602" s="7"/>
       <c r="U602" s="7"/>
       <c r="V602" s="20" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="603" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -30571,7 +30571,7 @@
         <v>145</v>
       </c>
       <c r="N607" s="20" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="O607" s="6"/>
       <c r="P607" s="7" t="s">
@@ -30583,7 +30583,7 @@
       <c r="T607" s="7"/>
       <c r="U607" s="7"/>
       <c r="V607" s="20" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="608" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -30904,7 +30904,7 @@
         <v>153</v>
       </c>
       <c r="N615" s="50" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="O615" s="6"/>
       <c r="P615" s="7" t="s">
@@ -30917,7 +30917,7 @@
         <v>120</v>
       </c>
       <c r="V615" s="20" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="616" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -31114,7 +31114,7 @@
         <v>158</v>
       </c>
       <c r="N620" s="20" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="O620" s="6"/>
       <c r="P620" s="7" t="s">
@@ -31126,7 +31126,7 @@
       <c r="T620" s="7"/>
       <c r="U620" s="7"/>
       <c r="V620" s="20" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="621" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -31454,7 +31454,7 @@
         <v>516</v>
       </c>
       <c r="O628" s="45" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="P628" s="7" t="s">
         <v>18</v>
@@ -31832,7 +31832,7 @@
         <v>175</v>
       </c>
       <c r="N637" s="20" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="O637" s="6"/>
       <c r="P637" s="7" t="s">
@@ -31844,7 +31844,7 @@
       <c r="T637" s="7"/>
       <c r="U637" s="7"/>
       <c r="V637" s="20" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="638" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -32168,7 +32168,7 @@
         <v>183</v>
       </c>
       <c r="N645" s="20" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="O645" s="7"/>
       <c r="P645" s="7" t="s">
@@ -32180,7 +32180,7 @@
       <c r="T645" s="7"/>
       <c r="U645" s="7"/>
       <c r="V645" s="20" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="646" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -32463,7 +32463,7 @@
         <v>190</v>
       </c>
       <c r="N652" s="20" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="O652" s="6"/>
       <c r="P652" s="7" t="s">
@@ -32475,7 +32475,7 @@
       <c r="T652" s="7"/>
       <c r="U652" s="7"/>
       <c r="V652" s="20" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="653" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -32760,7 +32760,7 @@
         <v>197</v>
       </c>
       <c r="N659" s="20" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="O659" s="7" t="s">
         <v>0</v>
@@ -32774,7 +32774,7 @@
       <c r="T659" s="7"/>
       <c r="U659" s="7"/>
       <c r="V659" s="20" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="660" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -33072,7 +33072,7 @@
       <c r="T666" s="7"/>
       <c r="U666" s="7"/>
       <c r="V666" s="20" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="667" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -33326,7 +33326,7 @@
         <v>210</v>
       </c>
       <c r="N672" s="20" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="O672" s="6"/>
       <c r="P672" s="7" t="s">
@@ -33338,7 +33338,7 @@
       <c r="T672" s="7"/>
       <c r="U672" s="7"/>
       <c r="V672" s="20" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="673" spans="1:22" x14ac:dyDescent="0.25">
@@ -33682,7 +33682,7 @@
       <c r="T680" s="7"/>
       <c r="U680" s="7"/>
       <c r="V680" s="20" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="681" spans="1:22" x14ac:dyDescent="0.25">
@@ -33924,7 +33924,7 @@
         <v>224</v>
       </c>
       <c r="N686" s="20" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="O686" s="6" t="s">
         <v>17</v>
@@ -33938,7 +33938,7 @@
       <c r="T686" s="7"/>
       <c r="U686" s="7"/>
       <c r="V686" s="20" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="687" spans="1:22" x14ac:dyDescent="0.25">
@@ -34143,7 +34143,7 @@
         <v>229</v>
       </c>
       <c r="N691" s="20" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="O691" s="6"/>
       <c r="P691" s="7" t="s">
@@ -34155,7 +34155,7 @@
       <c r="T691" s="7"/>
       <c r="U691" s="7"/>
       <c r="V691" s="20" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="692" spans="1:22" x14ac:dyDescent="0.25">
@@ -34448,7 +34448,7 @@
         <v>236</v>
       </c>
       <c r="N698" s="20" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="O698" s="6"/>
       <c r="P698" s="7" t="s">
@@ -34460,7 +34460,7 @@
       <c r="T698" s="7"/>
       <c r="U698" s="7"/>
       <c r="V698" s="20" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="699" spans="1:22" x14ac:dyDescent="0.25">
@@ -34624,7 +34624,7 @@
         <v>240</v>
       </c>
       <c r="N702" s="20" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="O702" s="6"/>
       <c r="P702" s="7" t="s">
@@ -34636,7 +34636,7 @@
       <c r="T702" s="7"/>
       <c r="U702" s="7"/>
       <c r="V702" s="20" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="703" spans="1:22" x14ac:dyDescent="0.25">
@@ -34956,7 +34956,7 @@
         <v>248</v>
       </c>
       <c r="N710" s="20" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="O710" s="6"/>
       <c r="P710" s="7" t="s">
@@ -34968,7 +34968,7 @@
       <c r="T710" s="7"/>
       <c r="U710" s="7"/>
       <c r="V710" s="20" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="711" spans="1:22" x14ac:dyDescent="0.25">
@@ -35182,7 +35182,7 @@
       <c r="T715" s="7"/>
       <c r="U715" s="7"/>
       <c r="V715" s="20" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="716" spans="1:22" x14ac:dyDescent="0.25">
@@ -35469,7 +35469,7 @@
         <v>260</v>
       </c>
       <c r="N722" s="20" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="O722" s="6"/>
       <c r="P722" s="7" t="s">
@@ -35481,7 +35481,7 @@
       <c r="T722" s="7"/>
       <c r="U722" s="7"/>
       <c r="V722" s="20" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="723" spans="1:22" x14ac:dyDescent="0.25">
@@ -35987,7 +35987,7 @@
         <v>272</v>
       </c>
       <c r="N734" s="20" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="O734" s="6"/>
       <c r="P734" s="7" t="s">
@@ -35999,7 +35999,7 @@
       <c r="T734" s="7"/>
       <c r="U734" s="7"/>
       <c r="V734" s="16" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="735" spans="1:22" x14ac:dyDescent="0.25">
@@ -36353,7 +36353,7 @@
       <c r="T742" s="7"/>
       <c r="U742" s="7"/>
       <c r="V742" s="20" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="743" spans="1:22" x14ac:dyDescent="0.25">
@@ -36769,7 +36769,7 @@
         <v>290</v>
       </c>
       <c r="N752" s="20" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="O752" s="6"/>
       <c r="P752" s="7" t="s">
@@ -36781,7 +36781,7 @@
       <c r="T752" s="7"/>
       <c r="U752" s="7"/>
       <c r="V752" s="20" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="753" spans="1:22" x14ac:dyDescent="0.25">
@@ -37031,7 +37031,7 @@
         <v>296</v>
       </c>
       <c r="N758" s="20" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="O758" s="6"/>
       <c r="P758" s="7" t="s">
@@ -37043,7 +37043,7 @@
       <c r="T758" s="7"/>
       <c r="U758" s="7"/>
       <c r="V758" s="20" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="759" spans="1:22" x14ac:dyDescent="0.25">
@@ -37513,7 +37513,7 @@
         <v>307</v>
       </c>
       <c r="N769" s="20" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="O769" s="6"/>
       <c r="P769" s="7" t="s">
@@ -37525,7 +37525,7 @@
       <c r="T769" s="7"/>
       <c r="U769" s="7"/>
       <c r="V769" s="16" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="770" spans="1:22" x14ac:dyDescent="0.25">
@@ -37943,7 +37943,7 @@
         <v>317</v>
       </c>
       <c r="N779" s="20" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="O779" s="7" t="s">
         <v>0</v>
@@ -37957,7 +37957,7 @@
       <c r="T779" s="7"/>
       <c r="U779" s="7"/>
       <c r="V779" s="20" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="780" spans="1:22" x14ac:dyDescent="0.25">
@@ -38074,7 +38074,7 @@
         <v>320</v>
       </c>
       <c r="N782" s="20" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="O782" s="7"/>
       <c r="P782" s="7" t="s">
@@ -38086,7 +38086,7 @@
       <c r="T782" s="7"/>
       <c r="U782" s="7"/>
       <c r="V782" s="20" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="783" spans="1:22" x14ac:dyDescent="0.25">
@@ -38381,7 +38381,7 @@
         <v>327</v>
       </c>
       <c r="N789" s="20" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="O789" s="7"/>
       <c r="P789" s="7" t="s">
@@ -38393,7 +38393,7 @@
       <c r="T789" s="7"/>
       <c r="U789" s="7"/>
       <c r="V789" s="20" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="790" spans="1:22" x14ac:dyDescent="0.25">
@@ -38549,7 +38549,7 @@
         <v>331</v>
       </c>
       <c r="N793" s="20" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="O793" s="6"/>
       <c r="P793" s="7" t="s">
@@ -38559,7 +38559,7 @@
       <c r="R793" s="7"/>
       <c r="U793" s="7"/>
       <c r="V793" s="20" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="794" spans="1:22" x14ac:dyDescent="0.25">
@@ -38856,7 +38856,7 @@
         <v>338</v>
       </c>
       <c r="N800" s="20" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="O800" s="6"/>
       <c r="P800" s="7" t="s">
@@ -38868,7 +38868,7 @@
       <c r="T800" s="7"/>
       <c r="U800" s="7"/>
       <c r="V800" s="20" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="801" spans="1:22" x14ac:dyDescent="0.25">
@@ -39108,7 +39108,7 @@
         <v>344</v>
       </c>
       <c r="N806" s="20" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="O806" s="6"/>
       <c r="P806" s="7" t="s">
@@ -39120,7 +39120,7 @@
       <c r="T806" s="7"/>
       <c r="U806" s="7"/>
       <c r="V806" s="20" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="807" spans="1:22" x14ac:dyDescent="0.25">
@@ -39502,7 +39502,7 @@
       <c r="T815" s="7"/>
       <c r="U815" s="7"/>
       <c r="V815" s="20" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="816" spans="1:22" x14ac:dyDescent="0.25">
@@ -39662,7 +39662,7 @@
         <v>357</v>
       </c>
       <c r="N819" s="20" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="O819" s="6"/>
       <c r="P819" s="7" t="s">
@@ -39674,7 +39674,7 @@
       <c r="T819" s="7"/>
       <c r="U819" s="7"/>
       <c r="V819" s="20" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="820" spans="1:22" x14ac:dyDescent="0.25">
@@ -39994,7 +39994,7 @@
         <v>365</v>
       </c>
       <c r="N827" s="20" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="O827" s="7" t="s">
         <v>0</v>
@@ -40008,7 +40008,7 @@
       <c r="T827" s="7"/>
       <c r="U827" s="7"/>
       <c r="V827" s="20" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="828" spans="1:22" x14ac:dyDescent="0.25">
@@ -40123,7 +40123,7 @@
         <v>368</v>
       </c>
       <c r="N830" s="20" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="O830" s="7" t="s">
         <v>0</v>
@@ -40137,7 +40137,7 @@
       <c r="T830" s="7"/>
       <c r="U830" s="7"/>
       <c r="V830" s="20" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="831" spans="1:22" x14ac:dyDescent="0.25">
@@ -40379,7 +40379,7 @@
         <v>374</v>
       </c>
       <c r="N836" s="20" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="O836" s="6"/>
       <c r="P836" s="7" t="s">
@@ -40391,7 +40391,7 @@
       <c r="T836" s="7"/>
       <c r="U836" s="7"/>
       <c r="V836" s="20" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="837" spans="1:22" x14ac:dyDescent="0.25">
@@ -40484,7 +40484,7 @@
     </row>
     <row r="839" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A839" s="16" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="B839" s="28"/>
       <c r="C839" s="38" t="s">
@@ -40665,7 +40665,7 @@
       <c r="T842" s="7"/>
       <c r="U842" s="7"/>
       <c r="V842" s="20" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="843" spans="1:22" x14ac:dyDescent="0.25">
@@ -40837,7 +40837,7 @@
         <v>384</v>
       </c>
       <c r="N846" s="20" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="O846" s="7"/>
       <c r="P846" s="7" t="s">
@@ -40851,7 +40851,7 @@
         <v>119</v>
       </c>
       <c r="V846" s="20" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="847" spans="1:22" x14ac:dyDescent="0.25">
@@ -41048,7 +41048,7 @@
         <v>389</v>
       </c>
       <c r="N851" s="20" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="O851" s="6"/>
       <c r="P851" s="7" t="s">
@@ -41060,7 +41060,7 @@
       <c r="T851" s="7"/>
       <c r="U851" s="7"/>
       <c r="V851" s="20" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="852" spans="1:22" x14ac:dyDescent="0.25">
@@ -41216,7 +41216,7 @@
         <v>393</v>
       </c>
       <c r="N855" s="20" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="O855" s="6"/>
       <c r="P855" s="7" t="s">
@@ -41228,7 +41228,7 @@
       <c r="T855" s="7"/>
       <c r="U855" s="7"/>
       <c r="V855" s="20" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="856" spans="1:22" x14ac:dyDescent="0.25">
@@ -41384,7 +41384,7 @@
         <v>397</v>
       </c>
       <c r="N859" s="20" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="O859" s="7" t="s">
         <v>0</v>
@@ -41398,7 +41398,7 @@
       <c r="T859" s="7"/>
       <c r="U859" s="7"/>
       <c r="V859" s="20" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="860" spans="1:22" x14ac:dyDescent="0.25">
@@ -41513,7 +41513,7 @@
         <v>400</v>
       </c>
       <c r="N862" s="20" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="O862" s="7" t="s">
         <v>0</v>
@@ -41527,7 +41527,7 @@
       <c r="T862" s="7"/>
       <c r="U862" s="7"/>
       <c r="V862" s="20" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="863" spans="1:22" x14ac:dyDescent="0.25">
@@ -41732,7 +41732,7 @@
         <v>405</v>
       </c>
       <c r="N867" s="20" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="O867" s="6"/>
       <c r="P867" s="7" t="s">
@@ -41744,7 +41744,7 @@
       <c r="T867" s="7"/>
       <c r="U867" s="7"/>
       <c r="V867" s="20" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="868" spans="1:22" x14ac:dyDescent="0.25">
@@ -45637,7 +45637,7 @@
       <c r="T965" s="7"/>
       <c r="U965" s="7"/>
       <c r="V965" s="20" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="966" spans="1:22" x14ac:dyDescent="0.25">
@@ -50795,7 +50795,7 @@
       <c r="T1094" s="7"/>
       <c r="U1094" s="7"/>
       <c r="V1094" s="20" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="1095" spans="1:22" x14ac:dyDescent="0.25">
@@ -52948,7 +52948,7 @@
     </row>
     <row r="1148" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1148" s="7" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="B1148" s="28"/>
       <c r="C1148" s="28"/>
@@ -54110,7 +54110,7 @@
         <v>82</v>
       </c>
       <c r="N1176" s="20" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="O1176" s="7" t="s">
         <v>0</v>
@@ -54124,7 +54124,7 @@
       <c r="T1176" s="7"/>
       <c r="U1176" s="7"/>
       <c r="V1176" s="20" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="1177" spans="1:22" x14ac:dyDescent="0.25">
@@ -56091,7 +56091,7 @@
         <v>49</v>
       </c>
       <c r="N1225" s="20" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="O1225" s="6"/>
       <c r="P1225" s="7" t="s">
@@ -56103,7 +56103,7 @@
       <c r="T1225" s="7"/>
       <c r="U1225" s="7"/>
       <c r="V1225" s="20" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="1226" spans="1:22" x14ac:dyDescent="0.25">
@@ -59050,7 +59050,7 @@
         <v>71</v>
       </c>
       <c r="N1296" s="20" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="O1296" s="6"/>
       <c r="P1296" s="7" t="s">
@@ -59062,7 +59062,7 @@
       <c r="T1296" s="7"/>
       <c r="U1296" s="7"/>
       <c r="V1296" s="20" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="1297" spans="1:22" x14ac:dyDescent="0.25">
@@ -61863,8 +61863,8 @@
       <c r="S1367" s="7"/>
       <c r="T1367" s="7"/>
       <c r="U1367" s="7"/>
-      <c r="V1367" s="20" t="s">
-        <v>1323</v>
+      <c r="V1367" s="16" t="s">
+        <v>1555</v>
       </c>
     </row>
     <row r="1368" spans="1:22" x14ac:dyDescent="0.25">
@@ -61946,7 +61946,7 @@
       <c r="T1369" s="7"/>
       <c r="U1369" s="7"/>
       <c r="V1369" s="20" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="1370" spans="1:22" x14ac:dyDescent="0.25">
@@ -62262,7 +62262,7 @@
       <c r="T1377" s="7"/>
       <c r="U1377" s="7"/>
       <c r="V1377" s="20" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="1378" spans="1:22" x14ac:dyDescent="0.25">
@@ -63084,7 +63084,7 @@
       <c r="T1398" s="7"/>
       <c r="U1398" s="7"/>
       <c r="V1398" s="20" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="1399" spans="1:22" x14ac:dyDescent="0.25">
@@ -63244,7 +63244,7 @@
       <c r="T1402" s="7"/>
       <c r="U1402" s="7"/>
       <c r="V1402" s="20" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="1403" spans="1:22" x14ac:dyDescent="0.25">
@@ -63365,7 +63365,7 @@
       <c r="T1405" s="7"/>
       <c r="U1405" s="7"/>
       <c r="V1405" s="20" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="1406" spans="1:22" x14ac:dyDescent="0.25">
@@ -63447,7 +63447,7 @@
       <c r="T1407" s="7"/>
       <c r="U1407" s="7"/>
       <c r="V1407" s="20" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="1408" spans="1:22" x14ac:dyDescent="0.25">
@@ -63802,7 +63802,7 @@
       <c r="T1416" s="7"/>
       <c r="U1416" s="7"/>
       <c r="V1416" s="20" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="1417" spans="1:22" x14ac:dyDescent="0.25">
@@ -63962,7 +63962,7 @@
       <c r="T1420" s="7"/>
       <c r="U1420" s="7"/>
       <c r="V1420" s="20" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="1421" spans="1:22" x14ac:dyDescent="0.25">
@@ -64307,7 +64307,7 @@
         <v>133</v>
       </c>
       <c r="N1429" s="20" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="O1429" s="6"/>
       <c r="P1429" s="7" t="s">
@@ -64319,7 +64319,7 @@
       <c r="T1429" s="7"/>
       <c r="U1429" s="7"/>
       <c r="V1429" s="20" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="1430" spans="1:22" x14ac:dyDescent="0.25">
@@ -64554,8 +64554,8 @@
       <c r="S1435" s="7"/>
       <c r="T1435" s="7"/>
       <c r="U1435" s="7"/>
-      <c r="V1435" s="20" t="s">
-        <v>1331</v>
+      <c r="V1435" s="16" t="s">
+        <v>1554</v>
       </c>
     </row>
     <row r="1436" spans="1:22" x14ac:dyDescent="0.25">
@@ -64792,8 +64792,8 @@
       <c r="S1441" s="7"/>
       <c r="T1441" s="7"/>
       <c r="U1441" s="7"/>
-      <c r="V1441" s="20" t="s">
-        <v>1331</v>
+      <c r="V1441" s="16" t="s">
+        <v>1554</v>
       </c>
     </row>
     <row r="1442" spans="1:22" x14ac:dyDescent="0.25">
@@ -65030,8 +65030,8 @@
       <c r="S1447" s="7"/>
       <c r="T1447" s="7"/>
       <c r="U1447" s="7"/>
-      <c r="V1447" s="20" t="s">
-        <v>1331</v>
+      <c r="V1447" s="16" t="s">
+        <v>1554</v>
       </c>
     </row>
     <row r="1448" spans="1:22" x14ac:dyDescent="0.25">
@@ -65268,8 +65268,8 @@
       <c r="S1453" s="7"/>
       <c r="T1453" s="7"/>
       <c r="U1453" s="7"/>
-      <c r="V1453" s="20" t="s">
-        <v>1331</v>
+      <c r="V1453" s="16" t="s">
+        <v>1554</v>
       </c>
     </row>
     <row r="1454" spans="1:22" x14ac:dyDescent="0.25">
@@ -65506,8 +65506,8 @@
       <c r="S1459" s="7"/>
       <c r="T1459" s="7"/>
       <c r="U1459" s="7"/>
-      <c r="V1459" s="20" t="s">
-        <v>1331</v>
+      <c r="V1459" s="16" t="s">
+        <v>1554</v>
       </c>
     </row>
     <row r="1460" spans="1:22" x14ac:dyDescent="0.25">
@@ -65744,8 +65744,8 @@
       <c r="S1465" s="7"/>
       <c r="T1465" s="7"/>
       <c r="U1465" s="7"/>
-      <c r="V1465" s="20" t="s">
-        <v>1331</v>
+      <c r="V1465" s="16" t="s">
+        <v>1554</v>
       </c>
     </row>
     <row r="1466" spans="1:22" x14ac:dyDescent="0.25">
@@ -65827,7 +65827,7 @@
       <c r="T1467" s="7"/>
       <c r="U1467" s="7"/>
       <c r="V1467" s="20" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="1468" spans="1:22" x14ac:dyDescent="0.25">
@@ -65948,7 +65948,7 @@
       <c r="T1470" s="7"/>
       <c r="U1470" s="7"/>
       <c r="V1470" s="20" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="1471" spans="1:22" x14ac:dyDescent="0.25">
@@ -66252,7 +66252,7 @@
         <v>49</v>
       </c>
       <c r="N1478" s="20" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="O1478" s="6"/>
       <c r="P1478" s="7"/>
@@ -66303,7 +66303,7 @@
       <c r="T1479" s="7"/>
       <c r="U1479" s="7"/>
       <c r="V1479" s="20" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="1480" spans="1:22" x14ac:dyDescent="0.25">
@@ -66423,7 +66423,7 @@
       <c r="T1482" s="7"/>
       <c r="U1482" s="7"/>
       <c r="V1482" s="20" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="1483" spans="1:22" x14ac:dyDescent="0.25">
@@ -66505,7 +66505,7 @@
       <c r="T1484" s="7"/>
       <c r="U1484" s="7"/>
       <c r="V1484" s="20" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="1485" spans="1:22" x14ac:dyDescent="0.25">
@@ -66592,8 +66592,8 @@
       <c r="S1486" s="7"/>
       <c r="T1486" s="7"/>
       <c r="U1486" s="7"/>
-      <c r="V1486" s="20" t="s">
-        <v>1331</v>
+      <c r="V1486" s="16" t="s">
+        <v>1554</v>
       </c>
     </row>
     <row r="1487" spans="1:22" x14ac:dyDescent="0.25">
@@ -66960,7 +66960,7 @@
       <c r="T1495" s="7"/>
       <c r="U1495" s="7"/>
       <c r="V1495" s="20" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="1496" spans="1:22" x14ac:dyDescent="0.25">
@@ -67042,7 +67042,7 @@
       <c r="T1497" s="7"/>
       <c r="U1497" s="7"/>
       <c r="V1497" s="20" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="1498" spans="1:22" x14ac:dyDescent="0.25">
@@ -67982,7 +67982,7 @@
       <c r="T1521" s="7"/>
       <c r="U1521" s="7"/>
       <c r="V1521" s="20" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="1522" spans="1:22" x14ac:dyDescent="0.25">
@@ -69065,7 +69065,7 @@
       <c r="T1551" s="7"/>
       <c r="U1551" s="7"/>
       <c r="V1551" s="20" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="1552" spans="1:22" x14ac:dyDescent="0.25">
@@ -69164,7 +69164,7 @@
       <c r="T1554" s="7"/>
       <c r="U1554" s="7"/>
       <c r="V1554" s="20" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="1555" spans="5:22" x14ac:dyDescent="0.25">
@@ -69263,7 +69263,7 @@
       <c r="T1557" s="7"/>
       <c r="U1557" s="7"/>
       <c r="V1557" s="20" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="1558" spans="5:22" x14ac:dyDescent="0.25">
@@ -69362,7 +69362,7 @@
       <c r="T1560" s="7"/>
       <c r="U1560" s="7"/>
       <c r="V1560" s="20" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="1561" spans="5:22" x14ac:dyDescent="0.25">
@@ -69990,7 +69990,7 @@
       <c r="T1580" s="7"/>
       <c r="U1580" s="7"/>
       <c r="V1580" s="20" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="1581" spans="9:22" x14ac:dyDescent="0.25">
@@ -70043,7 +70043,7 @@
         <v>0</v>
       </c>
       <c r="V1582" s="20" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1583" spans="9:22" x14ac:dyDescent="0.25">
@@ -70144,7 +70144,7 @@
         <v>0</v>
       </c>
       <c r="V1586" s="20" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="1587" spans="9:22" x14ac:dyDescent="0.25">
@@ -70343,7 +70343,7 @@
         <v>0</v>
       </c>
       <c r="V1594" s="20" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="1595" spans="9:22" x14ac:dyDescent="0.25">
@@ -70645,7 +70645,7 @@
         <v>0</v>
       </c>
       <c r="V1606" s="20" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="1607" spans="8:22" x14ac:dyDescent="0.25">
@@ -70704,7 +70704,7 @@
         <v>0</v>
       </c>
       <c r="V1608" s="20" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="1609" spans="8:22" x14ac:dyDescent="0.25">
@@ -70733,7 +70733,7 @@
         <v>0</v>
       </c>
       <c r="V1609" s="20" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="1610" spans="8:22" x14ac:dyDescent="0.25">
@@ -70762,7 +70762,7 @@
         <v>0</v>
       </c>
       <c r="V1610" s="20" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="1611" spans="8:22" x14ac:dyDescent="0.25">
@@ -70815,7 +70815,7 @@
         <v>0</v>
       </c>
       <c r="V1612" s="20" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="1613" spans="8:22" x14ac:dyDescent="0.25">
@@ -70991,7 +70991,7 @@
         <v>0</v>
       </c>
       <c r="V1619" s="20" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="1620" spans="1:22" x14ac:dyDescent="0.25">
@@ -71044,7 +71044,7 @@
         <v>0</v>
       </c>
       <c r="V1621" s="20" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="1622" spans="1:22" x14ac:dyDescent="0.25">
@@ -71124,7 +71124,7 @@
         <v>18</v>
       </c>
       <c r="V1624" s="20" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="1625" spans="1:22" x14ac:dyDescent="0.25">
@@ -71157,7 +71157,7 @@
         <v>0</v>
       </c>
       <c r="V1625" s="20" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="1626" spans="1:22" x14ac:dyDescent="0.25">
@@ -71279,7 +71279,7 @@
         <v>0</v>
       </c>
       <c r="V1629" s="20" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="1630" spans="1:22" x14ac:dyDescent="0.25">
@@ -71419,7 +71419,7 @@
         <v>18</v>
       </c>
       <c r="V1634" s="20" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="1635" spans="3:22" x14ac:dyDescent="0.25">
@@ -71673,7 +71673,7 @@
         <v>18</v>
       </c>
       <c r="V1643" s="20" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="1644" spans="3:22" x14ac:dyDescent="0.25">
@@ -71737,7 +71737,7 @@
         <v>0</v>
       </c>
       <c r="V1645" s="20" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="1646" spans="3:22" x14ac:dyDescent="0.25">
@@ -71871,7 +71871,7 @@
         <v>26</v>
       </c>
       <c r="N1650" s="20" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="O1650" s="7" t="s">
         <v>0</v>
@@ -71880,7 +71880,7 @@
         <v>18</v>
       </c>
       <c r="V1650" s="20" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="1651" spans="3:22" x14ac:dyDescent="0.25">
@@ -71971,7 +71971,7 @@
         <v>0</v>
       </c>
       <c r="V1653" s="20" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="1654" spans="3:22" x14ac:dyDescent="0.25">
@@ -72162,13 +72162,13 @@
         <v>36</v>
       </c>
       <c r="N1660" s="20" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="P1660" s="7" t="s">
         <v>18</v>
       </c>
       <c r="V1660" s="20" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="1661" spans="3:22" x14ac:dyDescent="0.25">
@@ -72254,7 +72254,7 @@
         <v>0</v>
       </c>
       <c r="V1663" s="20" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="1664" spans="3:22" x14ac:dyDescent="0.25">
@@ -72396,13 +72396,13 @@
         <v>44</v>
       </c>
       <c r="N1668" s="20" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="P1668" s="7" t="s">
         <v>18</v>
       </c>
       <c r="V1668" s="20" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="1669" spans="3:22" x14ac:dyDescent="0.25">
@@ -72690,7 +72690,7 @@
         <v>18</v>
       </c>
       <c r="V1678" s="20" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="1679" spans="3:22" x14ac:dyDescent="0.25">
@@ -72776,7 +72776,7 @@
         <v>0</v>
       </c>
       <c r="V1681" s="20" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="1682" spans="3:22" x14ac:dyDescent="0.25">
@@ -72808,7 +72808,7 @@
         <v>0</v>
       </c>
       <c r="V1682" s="20" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="1683" spans="3:22" x14ac:dyDescent="0.25">
@@ -72915,7 +72915,7 @@
         <v>62</v>
       </c>
       <c r="N1686" s="20" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="O1686" s="7" t="s">
         <v>0</v>
@@ -72924,7 +72924,7 @@
         <v>18</v>
       </c>
       <c r="V1686" s="20" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="1687" spans="3:22" x14ac:dyDescent="0.25">
@@ -73010,7 +73010,7 @@
         <v>0</v>
       </c>
       <c r="V1689" s="20" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="1690" spans="3:22" x14ac:dyDescent="0.25">
@@ -73144,13 +73144,13 @@
         <v>70</v>
       </c>
       <c r="N1694" s="20" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="P1694" s="7" t="s">
         <v>18</v>
       </c>
       <c r="V1694" s="20" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="1695" spans="3:22" x14ac:dyDescent="0.25">
@@ -73236,7 +73236,7 @@
         <v>0</v>
       </c>
       <c r="V1697" s="20" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="1698" spans="3:22" x14ac:dyDescent="0.25">
@@ -73406,7 +73406,7 @@
         <v>18</v>
       </c>
       <c r="V1703" s="20" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="1704" spans="3:22" x14ac:dyDescent="0.25">
@@ -73576,7 +73576,7 @@
         <v>0</v>
       </c>
       <c r="V1709" s="20" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="1710" spans="3:22" x14ac:dyDescent="0.25">
@@ -73629,13 +73629,13 @@
         <v>87</v>
       </c>
       <c r="N1711" s="20" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="P1711" s="7" t="s">
         <v>18</v>
       </c>
       <c r="V1711" s="20" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="1712" spans="3:22" x14ac:dyDescent="0.25">
@@ -73907,13 +73907,13 @@
         <v>97</v>
       </c>
       <c r="N1721" s="20" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="P1721" s="7" t="s">
         <v>18</v>
       </c>
       <c r="V1721" s="20" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="1722" spans="3:22" x14ac:dyDescent="0.25">
@@ -73999,7 +73999,7 @@
         <v>0</v>
       </c>
       <c r="V1724" s="20" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="1725" spans="3:22" x14ac:dyDescent="0.25">
@@ -74111,7 +74111,7 @@
         <v>0</v>
       </c>
       <c r="V1728" s="20" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="1729" spans="3:22" x14ac:dyDescent="0.25">
@@ -74137,13 +74137,13 @@
         <v>105</v>
       </c>
       <c r="N1729" s="20" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="P1729" s="7" t="s">
         <v>18</v>
       </c>
       <c r="V1729" s="20" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="1730" spans="3:22" x14ac:dyDescent="0.25">
@@ -74310,7 +74310,7 @@
         <v>0</v>
       </c>
       <c r="V1735" s="20" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="1736" spans="3:22" x14ac:dyDescent="0.25">
@@ -74369,7 +74369,7 @@
         <v>0</v>
       </c>
       <c r="V1737" s="20" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="1738" spans="3:22" x14ac:dyDescent="0.25">
@@ -74431,7 +74431,7 @@
         <v>18</v>
       </c>
       <c r="V1739" s="20" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="1740" spans="3:22" x14ac:dyDescent="0.25">
@@ -74463,7 +74463,7 @@
         <v>0</v>
       </c>
       <c r="V1740" s="20" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="1741" spans="3:22" x14ac:dyDescent="0.25">
@@ -74549,7 +74549,7 @@
         <v>17</v>
       </c>
       <c r="V1743" s="20" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="1744" spans="3:22" x14ac:dyDescent="0.25">
@@ -74683,13 +74683,13 @@
         <v>124</v>
       </c>
       <c r="N1748" s="20" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="P1748" s="7" t="s">
         <v>18</v>
       </c>
       <c r="V1748" s="20" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="1749" spans="3:22" x14ac:dyDescent="0.25">
@@ -74874,7 +74874,7 @@
         <v>0</v>
       </c>
       <c r="V1754" s="20" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="1755" spans="3:22" x14ac:dyDescent="0.25">
@@ -74906,7 +74906,7 @@
         <v>0</v>
       </c>
       <c r="V1755" s="20" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="1756" spans="3:22" x14ac:dyDescent="0.25">
@@ -74965,7 +74965,7 @@
         <v>18</v>
       </c>
       <c r="V1757" s="20" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="1758" spans="3:22" x14ac:dyDescent="0.25">
@@ -75051,7 +75051,7 @@
         <v>0</v>
       </c>
       <c r="V1760" s="20" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="1761" spans="3:22" x14ac:dyDescent="0.25">
@@ -75083,7 +75083,7 @@
         <v>0</v>
       </c>
       <c r="V1761" s="20" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="1762" spans="3:22" x14ac:dyDescent="0.25">
@@ -75115,7 +75115,7 @@
         <v>0</v>
       </c>
       <c r="V1762" s="20" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="1763" spans="3:22" x14ac:dyDescent="0.25">
@@ -75177,7 +75177,7 @@
         <v>18</v>
       </c>
       <c r="V1764" s="20" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="1765" spans="3:22" x14ac:dyDescent="0.25">
@@ -75209,7 +75209,7 @@
         <v>0</v>
       </c>
       <c r="V1765" s="20" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="1766" spans="3:22" x14ac:dyDescent="0.25">
@@ -75268,7 +75268,7 @@
         <v>0</v>
       </c>
       <c r="V1767" s="20" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="1768" spans="3:22" x14ac:dyDescent="0.25">
@@ -75381,7 +75381,7 @@
         <v>0</v>
       </c>
       <c r="V1771" s="20" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="1772" spans="3:22" x14ac:dyDescent="0.25">
@@ -75434,13 +75434,13 @@
         <v>149</v>
       </c>
       <c r="N1773" s="20" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="P1773" s="7" t="s">
         <v>18</v>
       </c>
       <c r="V1773" s="20" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="1774" spans="3:22" x14ac:dyDescent="0.25">
@@ -75472,7 +75472,7 @@
         <v>0</v>
       </c>
       <c r="V1774" s="20" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="1775" spans="3:22" x14ac:dyDescent="0.25">
@@ -75698,13 +75698,13 @@
         <v>158</v>
       </c>
       <c r="N1782" s="20" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="P1782" s="1" t="s">
         <v>18</v>
       </c>
       <c r="V1782" s="20" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="1783" spans="3:22" x14ac:dyDescent="0.25">
@@ -75736,7 +75736,7 @@
         <v>0</v>
       </c>
       <c r="V1783" s="20" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="1784" spans="3:22" x14ac:dyDescent="0.25">
@@ -75768,7 +75768,7 @@
         <v>0</v>
       </c>
       <c r="V1784" s="20" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="1785" spans="3:22" x14ac:dyDescent="0.25">
@@ -75977,7 +75977,7 @@
         <v>18</v>
       </c>
       <c r="V1791" s="20" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="1792" spans="3:22" x14ac:dyDescent="0.25">
@@ -76077,7 +76077,7 @@
         <v>0</v>
       </c>
       <c r="V1794" s="20" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="1795" spans="3:22" x14ac:dyDescent="0.25">
@@ -76244,13 +76244,13 @@
         <v>176</v>
       </c>
       <c r="N1800" s="20" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="P1800" s="7" t="s">
         <v>18</v>
       </c>
       <c r="V1800" s="20" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="1801" spans="3:22" x14ac:dyDescent="0.25">
@@ -76506,7 +76506,7 @@
         <v>119</v>
       </c>
       <c r="V1809" s="20" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="1810" spans="3:22" x14ac:dyDescent="0.25">
@@ -76601,7 +76601,7 @@
         <v>0</v>
       </c>
       <c r="V1812" s="16" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="1813" spans="3:22" x14ac:dyDescent="0.25">
@@ -76696,7 +76696,7 @@
         <v>0</v>
       </c>
       <c r="V1815" s="20" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="1816" spans="3:22" x14ac:dyDescent="0.25">
@@ -76785,7 +76785,7 @@
         <v>119</v>
       </c>
       <c r="V1818" s="20" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="1819" spans="3:22" x14ac:dyDescent="0.25">
@@ -76817,7 +76817,7 @@
         <v>0</v>
       </c>
       <c r="V1819" s="20" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="1820" spans="3:22" x14ac:dyDescent="0.25">
@@ -76903,7 +76903,7 @@
         <v>0</v>
       </c>
       <c r="V1822" s="20" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="1823" spans="3:22" x14ac:dyDescent="0.25">
@@ -76988,13 +76988,13 @@
         <v>201</v>
       </c>
       <c r="N1825" s="20" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="P1825" s="7" t="s">
         <v>18</v>
       </c>
       <c r="V1825" s="20" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="1826" spans="3:22" x14ac:dyDescent="0.25">
@@ -77026,7 +77026,7 @@
         <v>0</v>
       </c>
       <c r="V1826" s="20" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="1827" spans="3:22" x14ac:dyDescent="0.25">
@@ -77091,7 +77091,7 @@
         <v>0</v>
       </c>
       <c r="V1828" s="20" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="1829" spans="3:22" x14ac:dyDescent="0.25">
@@ -77249,7 +77249,7 @@
         <v>119</v>
       </c>
       <c r="V1833" s="20" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="1834" spans="3:22" x14ac:dyDescent="0.25">
@@ -77338,7 +77338,7 @@
         <v>0</v>
       </c>
       <c r="V1836" s="20" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="1837" spans="3:22" x14ac:dyDescent="0.25">
@@ -77511,13 +77511,13 @@
         <v>218</v>
       </c>
       <c r="N1842" s="20" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="P1842" s="7" t="s">
         <v>18</v>
       </c>
       <c r="V1842" s="20" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="1843" spans="3:22" x14ac:dyDescent="0.25">
@@ -77651,13 +77651,13 @@
         <v>223</v>
       </c>
       <c r="N1847" s="20" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="O1847" s="7" t="s">
         <v>0</v>
       </c>
       <c r="V1847" s="20" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="1848" spans="3:22" x14ac:dyDescent="0.25">
@@ -77770,13 +77770,13 @@
         <v>227</v>
       </c>
       <c r="N1851" s="20" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="P1851" s="7" t="s">
         <v>18</v>
       </c>
       <c r="V1851" s="20" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="1852" spans="3:22" x14ac:dyDescent="0.25">
@@ -78005,7 +78005,7 @@
         <v>18</v>
       </c>
       <c r="V1859" s="20" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="1860" spans="3:22" x14ac:dyDescent="0.25">
@@ -78096,7 +78096,7 @@
         <v>0</v>
       </c>
       <c r="V1862" s="20" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="1863" spans="3:22" x14ac:dyDescent="0.25">
@@ -78236,7 +78236,7 @@
         <v>243</v>
       </c>
       <c r="N1867" s="50" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="O1867" s="7" t="s">
         <v>0</v>
@@ -78245,7 +78245,7 @@
         <v>18</v>
       </c>
       <c r="V1867" s="20" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="1868" spans="3:22" x14ac:dyDescent="0.25">
@@ -78529,7 +78529,7 @@
         <v>0</v>
       </c>
       <c r="V1876" s="20" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="1877" spans="1:22" x14ac:dyDescent="0.25">
@@ -78627,7 +78627,7 @@
         <v>0</v>
       </c>
       <c r="V1879" s="20" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="1880" spans="1:22" x14ac:dyDescent="0.25">
@@ -78878,13 +78878,13 @@
         <v>264</v>
       </c>
       <c r="N1888" s="41" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="P1888" s="7" t="s">
         <v>18</v>
       </c>
       <c r="V1888" s="20" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nmv 24 03 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 4.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 4.4 Padam Input Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A08DB5-3E5F-46AE-B7B2-5E7143F7DFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BFFA04-6724-4142-B3F8-8D5826B1A2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4485,9 +4485,6 @@
     <t>janA#nAqmitiq janA#nAm</t>
   </si>
   <si>
-    <t>mIqDhuShaq iti# miqDhuSha#H</t>
-  </si>
-  <si>
     <t>naraq itiq nara#H</t>
   </si>
   <si>
@@ -4696,6 +4693,9 @@
   </si>
   <si>
     <t>sa(gm)sa$m</t>
+  </si>
+  <si>
+    <t>mIqDhuShaq iti# mIqDhuSha#H</t>
   </si>
 </sst>
 </file>
@@ -5318,10 +5318,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1888"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A608" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A672" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N621" sqref="N621"/>
+      <selection pane="bottomLeft" activeCell="P1901" sqref="P1901"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -13199,7 +13199,7 @@
         <v>40</v>
       </c>
       <c r="N184" s="16" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="O184" s="6"/>
       <c r="P184" s="7"/>
@@ -15323,7 +15323,7 @@
         <v>93</v>
       </c>
       <c r="N237" s="20" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="O237" s="7" t="s">
         <v>0</v>
@@ -15974,7 +15974,7 @@
       <c r="T253" s="7"/>
       <c r="U253" s="7"/>
       <c r="V253" s="16" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="254" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -16060,7 +16060,7 @@
       <c r="T255" s="7"/>
       <c r="U255" s="7"/>
       <c r="V255" s="16" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="256" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -18621,7 +18621,7 @@
         <v>34</v>
       </c>
       <c r="N318" s="20" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="O318" s="6"/>
       <c r="P318" s="7"/>
@@ -31162,7 +31162,7 @@
         <v>159</v>
       </c>
       <c r="N621" s="16" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="O621" s="7" t="s">
         <v>0</v>
@@ -31457,7 +31457,7 @@
         <v>515</v>
       </c>
       <c r="O628" s="45" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="P628" s="7" t="s">
         <v>18</v>
@@ -33340,8 +33340,8 @@
       <c r="S672" s="7"/>
       <c r="T672" s="7"/>
       <c r="U672" s="7"/>
-      <c r="V672" s="20" t="s">
-        <v>1485</v>
+      <c r="V672" s="16" t="s">
+        <v>1555</v>
       </c>
     </row>
     <row r="673" spans="1:22" x14ac:dyDescent="0.25">
@@ -33685,7 +33685,7 @@
       <c r="T680" s="7"/>
       <c r="U680" s="7"/>
       <c r="V680" s="20" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="681" spans="1:22" x14ac:dyDescent="0.25">
@@ -33941,7 +33941,7 @@
       <c r="T686" s="7"/>
       <c r="U686" s="7"/>
       <c r="V686" s="20" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="687" spans="1:22" x14ac:dyDescent="0.25">
@@ -34158,7 +34158,7 @@
       <c r="T691" s="7"/>
       <c r="U691" s="7"/>
       <c r="V691" s="20" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="692" spans="1:22" x14ac:dyDescent="0.25">
@@ -34463,7 +34463,7 @@
       <c r="T698" s="7"/>
       <c r="U698" s="7"/>
       <c r="V698" s="20" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="699" spans="1:22" x14ac:dyDescent="0.25">
@@ -34639,7 +34639,7 @@
       <c r="T702" s="7"/>
       <c r="U702" s="7"/>
       <c r="V702" s="20" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="703" spans="1:22" x14ac:dyDescent="0.25">
@@ -34971,7 +34971,7 @@
       <c r="T710" s="7"/>
       <c r="U710" s="7"/>
       <c r="V710" s="20" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="711" spans="1:22" x14ac:dyDescent="0.25">
@@ -35185,7 +35185,7 @@
       <c r="T715" s="7"/>
       <c r="U715" s="7"/>
       <c r="V715" s="20" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="716" spans="1:22" x14ac:dyDescent="0.25">
@@ -35484,7 +35484,7 @@
       <c r="T722" s="7"/>
       <c r="U722" s="7"/>
       <c r="V722" s="20" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="723" spans="1:22" x14ac:dyDescent="0.25">
@@ -36356,7 +36356,7 @@
       <c r="T742" s="7"/>
       <c r="U742" s="7"/>
       <c r="V742" s="20" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="743" spans="1:22" x14ac:dyDescent="0.25">
@@ -37046,7 +37046,7 @@
       <c r="T758" s="7"/>
       <c r="U758" s="7"/>
       <c r="V758" s="20" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="759" spans="1:22" x14ac:dyDescent="0.25">
@@ -37960,7 +37960,7 @@
       <c r="T779" s="7"/>
       <c r="U779" s="7"/>
       <c r="V779" s="20" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="780" spans="1:22" x14ac:dyDescent="0.25">
@@ -38089,7 +38089,7 @@
       <c r="T782" s="7"/>
       <c r="U782" s="7"/>
       <c r="V782" s="20" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="783" spans="1:22" x14ac:dyDescent="0.25">
@@ -38396,7 +38396,7 @@
       <c r="T789" s="7"/>
       <c r="U789" s="7"/>
       <c r="V789" s="20" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="790" spans="1:22" x14ac:dyDescent="0.25">
@@ -38562,7 +38562,7 @@
       <c r="R793" s="7"/>
       <c r="U793" s="7"/>
       <c r="V793" s="20" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="794" spans="1:22" x14ac:dyDescent="0.25">
@@ -38871,7 +38871,7 @@
       <c r="T800" s="7"/>
       <c r="U800" s="7"/>
       <c r="V800" s="20" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="801" spans="1:22" x14ac:dyDescent="0.25">
@@ -39123,7 +39123,7 @@
       <c r="T806" s="7"/>
       <c r="U806" s="7"/>
       <c r="V806" s="20" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="807" spans="1:22" x14ac:dyDescent="0.25">
@@ -39505,7 +39505,7 @@
       <c r="T815" s="7"/>
       <c r="U815" s="7"/>
       <c r="V815" s="20" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="816" spans="1:22" x14ac:dyDescent="0.25">
@@ -39677,7 +39677,7 @@
       <c r="T819" s="7"/>
       <c r="U819" s="7"/>
       <c r="V819" s="20" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="820" spans="1:22" x14ac:dyDescent="0.25">
@@ -40011,7 +40011,7 @@
       <c r="T827" s="7"/>
       <c r="U827" s="7"/>
       <c r="V827" s="20" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="828" spans="1:22" x14ac:dyDescent="0.25">
@@ -40140,7 +40140,7 @@
       <c r="T830" s="7"/>
       <c r="U830" s="7"/>
       <c r="V830" s="20" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="831" spans="1:22" x14ac:dyDescent="0.25">
@@ -40394,7 +40394,7 @@
       <c r="T836" s="7"/>
       <c r="U836" s="7"/>
       <c r="V836" s="20" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="837" spans="1:22" x14ac:dyDescent="0.25">
@@ -40487,7 +40487,7 @@
     </row>
     <row r="839" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A839" s="16" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="B839" s="28"/>
       <c r="C839" s="38" t="s">
@@ -40668,7 +40668,7 @@
       <c r="T842" s="7"/>
       <c r="U842" s="7"/>
       <c r="V842" s="20" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="843" spans="1:22" x14ac:dyDescent="0.25">
@@ -40854,7 +40854,7 @@
         <v>119</v>
       </c>
       <c r="V846" s="20" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="847" spans="1:22" x14ac:dyDescent="0.25">
@@ -41063,7 +41063,7 @@
       <c r="T851" s="7"/>
       <c r="U851" s="7"/>
       <c r="V851" s="20" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="852" spans="1:22" x14ac:dyDescent="0.25">
@@ -41231,7 +41231,7 @@
       <c r="T855" s="7"/>
       <c r="U855" s="7"/>
       <c r="V855" s="20" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="856" spans="1:22" x14ac:dyDescent="0.25">
@@ -41401,7 +41401,7 @@
       <c r="T859" s="7"/>
       <c r="U859" s="7"/>
       <c r="V859" s="20" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="860" spans="1:22" x14ac:dyDescent="0.25">
@@ -41530,7 +41530,7 @@
       <c r="T862" s="7"/>
       <c r="U862" s="7"/>
       <c r="V862" s="20" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="863" spans="1:22" x14ac:dyDescent="0.25">
@@ -41747,7 +41747,7 @@
       <c r="T867" s="7"/>
       <c r="U867" s="7"/>
       <c r="V867" s="20" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="868" spans="1:22" x14ac:dyDescent="0.25">
@@ -45640,7 +45640,7 @@
       <c r="T965" s="7"/>
       <c r="U965" s="7"/>
       <c r="V965" s="20" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="966" spans="1:22" x14ac:dyDescent="0.25">
@@ -52951,7 +52951,7 @@
     </row>
     <row r="1148" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1148" s="7" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="B1148" s="28"/>
       <c r="C1148" s="28"/>
@@ -54127,7 +54127,7 @@
       <c r="T1176" s="7"/>
       <c r="U1176" s="7"/>
       <c r="V1176" s="20" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="1177" spans="1:22" x14ac:dyDescent="0.25">
@@ -56106,7 +56106,7 @@
       <c r="T1225" s="7"/>
       <c r="U1225" s="7"/>
       <c r="V1225" s="20" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="1226" spans="1:22" x14ac:dyDescent="0.25">
@@ -59065,7 +59065,7 @@
       <c r="T1296" s="7"/>
       <c r="U1296" s="7"/>
       <c r="V1296" s="20" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="1297" spans="1:22" x14ac:dyDescent="0.25">
@@ -61867,7 +61867,7 @@
       <c r="T1367" s="7"/>
       <c r="U1367" s="7"/>
       <c r="V1367" s="16" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="1368" spans="1:22" x14ac:dyDescent="0.25">
@@ -64322,7 +64322,7 @@
       <c r="T1429" s="7"/>
       <c r="U1429" s="7"/>
       <c r="V1429" s="20" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="1430" spans="1:22" x14ac:dyDescent="0.25">
@@ -64558,7 +64558,7 @@
       <c r="T1435" s="7"/>
       <c r="U1435" s="7"/>
       <c r="V1435" s="16" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="1436" spans="1:22" x14ac:dyDescent="0.25">
@@ -64796,7 +64796,7 @@
       <c r="T1441" s="7"/>
       <c r="U1441" s="7"/>
       <c r="V1441" s="16" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="1442" spans="1:22" x14ac:dyDescent="0.25">
@@ -65034,7 +65034,7 @@
       <c r="T1447" s="7"/>
       <c r="U1447" s="7"/>
       <c r="V1447" s="16" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="1448" spans="1:22" x14ac:dyDescent="0.25">
@@ -65272,7 +65272,7 @@
       <c r="T1453" s="7"/>
       <c r="U1453" s="7"/>
       <c r="V1453" s="16" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="1454" spans="1:22" x14ac:dyDescent="0.25">
@@ -65510,7 +65510,7 @@
       <c r="T1459" s="7"/>
       <c r="U1459" s="7"/>
       <c r="V1459" s="16" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="1460" spans="1:22" x14ac:dyDescent="0.25">
@@ -65748,7 +65748,7 @@
       <c r="T1465" s="7"/>
       <c r="U1465" s="7"/>
       <c r="V1465" s="16" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="1466" spans="1:22" x14ac:dyDescent="0.25">
@@ -66255,7 +66255,7 @@
         <v>49</v>
       </c>
       <c r="N1478" s="20" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="O1478" s="6"/>
       <c r="P1478" s="7"/>
@@ -66596,7 +66596,7 @@
       <c r="T1486" s="7"/>
       <c r="U1486" s="7"/>
       <c r="V1486" s="16" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="1487" spans="1:22" x14ac:dyDescent="0.25">
@@ -71127,7 +71127,7 @@
         <v>18</v>
       </c>
       <c r="V1624" s="20" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="1625" spans="1:22" x14ac:dyDescent="0.25">
@@ -71425,7 +71425,7 @@
         <v>18</v>
       </c>
       <c r="V1634" s="20" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="1635" spans="3:22" x14ac:dyDescent="0.25">
@@ -71679,7 +71679,7 @@
         <v>18</v>
       </c>
       <c r="V1643" s="20" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="1644" spans="3:22" x14ac:dyDescent="0.25">
@@ -71886,7 +71886,7 @@
         <v>18</v>
       </c>
       <c r="V1650" s="20" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="1651" spans="3:22" x14ac:dyDescent="0.25">
@@ -72174,7 +72174,7 @@
         <v>18</v>
       </c>
       <c r="V1660" s="20" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="1661" spans="3:22" x14ac:dyDescent="0.25">
@@ -72408,7 +72408,7 @@
         <v>18</v>
       </c>
       <c r="V1668" s="20" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="1669" spans="3:22" x14ac:dyDescent="0.25">
@@ -72699,7 +72699,7 @@
         <v>18</v>
       </c>
       <c r="V1678" s="20" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="1679" spans="3:22" x14ac:dyDescent="0.25">
@@ -72924,7 +72924,7 @@
         <v>62</v>
       </c>
       <c r="N1686" s="16" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="O1686" s="7" t="s">
         <v>0</v>
@@ -72933,7 +72933,7 @@
         <v>18</v>
       </c>
       <c r="V1686" s="20" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="1687" spans="3:22" x14ac:dyDescent="0.25">
@@ -73159,7 +73159,7 @@
         <v>18</v>
       </c>
       <c r="V1694" s="20" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="1695" spans="3:22" x14ac:dyDescent="0.25">
@@ -73644,7 +73644,7 @@
         <v>18</v>
       </c>
       <c r="V1711" s="20" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="1712" spans="3:22" x14ac:dyDescent="0.25">
@@ -73922,7 +73922,7 @@
         <v>18</v>
       </c>
       <c r="V1721" s="20" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="1722" spans="3:22" x14ac:dyDescent="0.25">
@@ -74152,7 +74152,7 @@
         <v>18</v>
       </c>
       <c r="V1729" s="20" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="1730" spans="3:22" x14ac:dyDescent="0.25">
@@ -74440,7 +74440,7 @@
         <v>18</v>
       </c>
       <c r="V1739" s="20" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="1740" spans="3:22" x14ac:dyDescent="0.25">
@@ -74698,7 +74698,7 @@
         <v>18</v>
       </c>
       <c r="V1748" s="20" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="1749" spans="3:22" x14ac:dyDescent="0.25">
@@ -74974,7 +74974,7 @@
         <v>18</v>
       </c>
       <c r="V1757" s="20" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="1758" spans="3:22" x14ac:dyDescent="0.25">
@@ -75449,7 +75449,7 @@
         <v>18</v>
       </c>
       <c r="V1773" s="20" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="1774" spans="3:22" x14ac:dyDescent="0.25">
@@ -75713,7 +75713,7 @@
         <v>18</v>
       </c>
       <c r="V1782" s="20" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="1783" spans="3:22" x14ac:dyDescent="0.25">
@@ -75986,7 +75986,7 @@
         <v>18</v>
       </c>
       <c r="V1791" s="20" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="1792" spans="3:22" x14ac:dyDescent="0.25">
@@ -76259,7 +76259,7 @@
         <v>18</v>
       </c>
       <c r="V1800" s="20" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="1801" spans="3:22" x14ac:dyDescent="0.25">
@@ -76515,7 +76515,7 @@
         <v>119</v>
       </c>
       <c r="V1809" s="20" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="1810" spans="3:22" x14ac:dyDescent="0.25">
@@ -76794,7 +76794,7 @@
         <v>119</v>
       </c>
       <c r="V1818" s="20" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="1819" spans="3:22" x14ac:dyDescent="0.25">
@@ -77003,7 +77003,7 @@
         <v>18</v>
       </c>
       <c r="V1825" s="20" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="1826" spans="3:22" x14ac:dyDescent="0.25">
@@ -77258,7 +77258,7 @@
         <v>119</v>
       </c>
       <c r="V1833" s="20" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="1834" spans="3:22" x14ac:dyDescent="0.25">
@@ -77526,7 +77526,7 @@
         <v>18</v>
       </c>
       <c r="V1842" s="20" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="1843" spans="3:22" x14ac:dyDescent="0.25">
@@ -77660,13 +77660,13 @@
         <v>223</v>
       </c>
       <c r="N1847" s="20" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="O1847" s="7" t="s">
         <v>0</v>
       </c>
       <c r="V1847" s="20" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="1848" spans="3:22" x14ac:dyDescent="0.25">
@@ -77785,7 +77785,7 @@
         <v>18</v>
       </c>
       <c r="V1851" s="20" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="1852" spans="3:22" x14ac:dyDescent="0.25">
@@ -78254,7 +78254,7 @@
         <v>18</v>
       </c>
       <c r="V1867" s="20" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="1868" spans="3:22" x14ac:dyDescent="0.25">
@@ -78893,7 +78893,7 @@
         <v>18</v>
       </c>
       <c r="V1888" s="20" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>